<commit_message>
update color of xlsx
</commit_message>
<xml_diff>
--- a/doc/pr2_design/signal.xlsx
+++ b/doc/pr2_design/signal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="4890" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -224,7 +224,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,13 +239,27 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -257,14 +271,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="20" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="60% - 着色 4" xfId="1" builtinId="44"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -570,7 +590,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -612,20 +632,20 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -646,20 +666,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -677,17 +697,17 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
+    <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -705,17 +725,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
+    <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="3" t="s">
         <v>38</v>
       </c>
     </row>
@@ -733,17 +753,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11" t="s">
+    <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -761,17 +781,17 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" t="s">
+    <row r="13" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>